<commit_message>
DOVPROEV-6902 finalisatie eerste publicatie
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/bodemenondergrond/data/id/conceptscheme/bekistingsmateriaal/bekistingsmateriaal.xlsx
+++ b/src/main/resources/be/vlaanderen/bodemenondergrond/data/id/conceptscheme/bekistingsmateriaal/bekistingsmateriaal.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -425,9 +425,15 @@
         <v>prefLabel</v>
       </c>
       <c r="H1" t="str">
+        <v>definition</v>
+      </c>
+      <c r="I1" t="str">
+        <v>note</v>
+      </c>
+      <c r="J1" t="str">
         <v>topConceptOf</v>
       </c>
-      <c r="I1" t="str">
+      <c r="K1" t="str">
         <v>hasTopConcept</v>
       </c>
     </row>
@@ -445,7 +451,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
       </c>
       <c r="E2" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/0|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/10|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/11|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/12|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/1|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/2|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/3|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/4|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/5|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/6|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/7|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/8|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/9</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/0|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/1|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/2|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/3|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/4</v>
       </c>
       <c r="F2" t="str">
         <v>collectie_bekistingsmaterialen</v>
@@ -457,6 +463,12 @@
         <v>null</v>
       </c>
       <c r="I2" t="str">
+        <v>null</v>
+      </c>
+      <c r="J2" t="str">
+        <v>null</v>
+      </c>
+      <c r="K2" t="str">
         <v>null</v>
       </c>
     </row>
@@ -480,12 +492,18 @@
         <v>0</v>
       </c>
       <c r="G3" t="str">
-        <v>onbekend</v>
+        <v>natuurlijke materialen (biodegradeerbaar, hout, …)</v>
       </c>
       <c r="H3" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+        <v>Het boorgat is afgewerkt met natuurlijke materialen zoals bijvoorbeeld biologisch afbreekbare stoffen, hout.</v>
       </c>
       <c r="I3" t="str">
+        <v>Het boorgat is afgewerkt met natuurlijke materialen zoals bijvoorbeeld biologisch afbreekbare stoffen, hout.</v>
+      </c>
+      <c r="J3" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+      </c>
+      <c r="K3" t="str">
         <v>null</v>
       </c>
     </row>
@@ -509,24 +527,30 @@
         <v>1</v>
       </c>
       <c r="G4" t="str">
-        <v>PVC</v>
+        <v>kunststof: PVC</v>
       </c>
       <c r="H4" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+        <v>De materialen die in het boorgat achterblijven als al dan niet verloren bekisting of buizen bestaan uit PVC.</v>
       </c>
       <c r="I4" t="str">
+        <v>De materialen die in het boorgat achterblijven als al dan niet verloren bekisting of buizen bestaan uit PVC.</v>
+      </c>
+      <c r="J4" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+      </c>
+      <c r="K4" t="str">
         <v>null</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/10</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/2</v>
       </c>
       <c r="B5" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C5" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.10</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.2</v>
       </c>
       <c r="D5" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
@@ -535,27 +559,33 @@
         <v>null</v>
       </c>
       <c r="F5" t="str">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G5" t="str">
-        <v>metselwerk</v>
+        <v>kunststof: andere (PE, HDPE, LDPE, …)</v>
       </c>
       <c r="H5" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+        <v>De materialen die in het boorgat achterblijven als al dan niet verloren bekisting of buizen bestaan uit kunststof anders dan PVC zoals polyethylene (PE, HDPE, LDPE, …).</v>
       </c>
       <c r="I5" t="str">
+        <v>De materialen die in het boorgat achterblijven als al dan niet verloren bekisting of buizen bestaan uit kunststof anders dan PVC zoals polyethylene (PE, HDPE, LDPE, …).</v>
+      </c>
+      <c r="J5" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+      </c>
+      <c r="K5" t="str">
         <v>null</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/11</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/3</v>
       </c>
       <c r="B6" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C6" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.11</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.3</v>
       </c>
       <c r="D6" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
@@ -564,27 +594,33 @@
         <v>null</v>
       </c>
       <c r="F6" t="str">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G6" t="str">
-        <v>HDPE</v>
+        <v>metaal: inox, staal, roestvrij staal, gegalvaniseerd staal, …</v>
       </c>
       <c r="H6" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+        <v>De materialen die in het boorgat achterblijven als al dan niet verloren bekisting of buizen bestaan uit metaal zoals inox of staal.</v>
       </c>
       <c r="I6" t="str">
+        <v>De materialen die in het boorgat achterblijven als al dan niet verloren bekisting of buizen bestaan uit metaal zoals inox of staal.</v>
+      </c>
+      <c r="J6" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+      </c>
+      <c r="K6" t="str">
         <v>null</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/12</v>
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/4</v>
       </c>
       <c r="B7" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C7" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.12</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.4</v>
       </c>
       <c r="D7" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
@@ -593,282 +629,62 @@
         <v>null</v>
       </c>
       <c r="F7" t="str">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G7" t="str">
-        <v>straatpot</v>
+        <v>beton/metselwerk</v>
       </c>
       <c r="H7" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+        <v>Het boorgat is afgewerkt met bekisting uit beton of metselwerk.</v>
       </c>
       <c r="I7" t="str">
+        <v>Het boorgat is afgewerkt met bekisting uit beton of metselwerk.</v>
+      </c>
+      <c r="J7" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+      </c>
+      <c r="K7" t="str">
         <v>null</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/2</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
       </c>
       <c r="B8" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
       </c>
       <c r="C8" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.2</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.conceptscheme.bekistingsmateriaal</v>
       </c>
       <c r="D8" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+        <v>null</v>
       </c>
       <c r="E8" t="str">
         <v>null</v>
       </c>
       <c r="F8" t="str">
-        <v>2</v>
+        <v>bekistingsmaterialen</v>
       </c>
       <c r="G8" t="str">
-        <v>roestvrij staal</v>
+        <v>Conceptschema van bekistingsmaterialen.</v>
       </c>
       <c r="H8" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
+        <v>null</v>
       </c>
       <c r="I8" t="str">
         <v>null</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/3</v>
-      </c>
-      <c r="B9" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
-      </c>
-      <c r="C9" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.3</v>
-      </c>
-      <c r="D9" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="E9" t="str">
-        <v>null</v>
-      </c>
-      <c r="F9" t="str">
-        <v>3</v>
-      </c>
-      <c r="G9" t="str">
-        <v>gegalvaniseerd staal</v>
-      </c>
-      <c r="H9" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="I9" t="str">
-        <v>null</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/4</v>
-      </c>
-      <c r="B10" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
-      </c>
-      <c r="C10" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.4</v>
-      </c>
-      <c r="D10" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="E10" t="str">
-        <v>null</v>
-      </c>
-      <c r="F10" t="str">
-        <v>4</v>
-      </c>
-      <c r="G10" t="str">
-        <v>staal, zonder verdere precisering</v>
-      </c>
-      <c r="H10" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="I10" t="str">
-        <v>null</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/5</v>
-      </c>
-      <c r="B11" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
-      </c>
-      <c r="C11" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.5</v>
-      </c>
-      <c r="D11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="E11" t="str">
-        <v>null</v>
-      </c>
-      <c r="F11" t="str">
-        <v>5</v>
-      </c>
-      <c r="G11" t="str">
-        <v>glasvezel</v>
-      </c>
-      <c r="H11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="I11" t="str">
-        <v>null</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/6</v>
-      </c>
-      <c r="B12" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
-      </c>
-      <c r="C12" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.6</v>
-      </c>
-      <c r="D12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="E12" t="str">
-        <v>null</v>
-      </c>
-      <c r="F12" t="str">
-        <v>6</v>
-      </c>
-      <c r="G12" t="str">
-        <v>inox, zonder verdere precisering</v>
-      </c>
-      <c r="H12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="I12" t="str">
-        <v>null</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/7</v>
-      </c>
-      <c r="B13" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
-      </c>
-      <c r="C13" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.7</v>
-      </c>
-      <c r="D13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="E13" t="str">
-        <v>null</v>
-      </c>
-      <c r="F13" t="str">
-        <v>7</v>
-      </c>
-      <c r="G13" t="str">
-        <v>geen filterbuis aanwezig</v>
-      </c>
-      <c r="H13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="I13" t="str">
-        <v>null</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/8</v>
-      </c>
-      <c r="B14" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
-      </c>
-      <c r="C14" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.8</v>
-      </c>
-      <c r="D14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="E14" t="str">
-        <v>null</v>
-      </c>
-      <c r="F14" t="str">
-        <v>8</v>
-      </c>
-      <c r="G14" t="str">
-        <v>polyethyleen</v>
-      </c>
-      <c r="H14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="I14" t="str">
-        <v>null</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/9</v>
-      </c>
-      <c r="B15" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
-      </c>
-      <c r="C15" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.9</v>
-      </c>
-      <c r="D15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="E15" t="str">
-        <v>null</v>
-      </c>
-      <c r="F15" t="str">
-        <v>9</v>
-      </c>
-      <c r="G15" t="str">
-        <v>beton</v>
-      </c>
-      <c r="H15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="I15" t="str">
-        <v>null</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
-      </c>
-      <c r="B16" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
-      </c>
-      <c r="C16" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.conceptscheme.bekistingsmateriaal</v>
-      </c>
-      <c r="D16" t="str">
-        <v>null</v>
-      </c>
-      <c r="E16" t="str">
-        <v>null</v>
-      </c>
-      <c r="F16" t="str">
-        <v>bekistingsmaterialen</v>
-      </c>
-      <c r="G16" t="str">
-        <v>Conceptschema van bekistingsmaterialen.</v>
-      </c>
-      <c r="H16" t="str">
-        <v>null</v>
-      </c>
-      <c r="I16" t="str">
-        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/0|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/10|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/11|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/12|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/1|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/2|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/3|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/4|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/5|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/6|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/7|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/8|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/9</v>
+      <c r="J8" t="str">
+        <v>null</v>
+      </c>
+      <c r="K8" t="str">
+        <v>https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/0|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/1|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/2|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/3|https://data.bodemenondergrond.vlaanderen.be/id/concept/bekistingsmateriaal/4</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
foute codes gebruikt als dc.identifier
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/bodemenondergrond/data/id/conceptscheme/bekistingsmateriaal/bekistingsmateriaal.xlsx
+++ b/src/main/resources/be/vlaanderen/bodemenondergrond/data/id/conceptscheme/bekistingsmateriaal/bekistingsmateriaal.xlsx
@@ -550,7 +550,7 @@
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C5" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.3</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.metaal</v>
       </c>
       <c r="D5" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>
@@ -585,7 +585,7 @@
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C6" t="str">
-        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.0</v>
+        <v>be.vlaanderen.bodemenondergrond.data.id.concept.bekistingsmateriaal.natuurlijk</v>
       </c>
       <c r="D6" t="str">
         <v>https://data.bodemenondergrond.vlaanderen.be/id/conceptscheme/bekistingsmateriaal</v>

</xml_diff>